<commit_message>
add sure as a function
</commit_message>
<xml_diff>
--- a/Test Excel.xlsx
+++ b/Test Excel.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,9 +49,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -477,6 +479,23 @@
       </c>
       <c r="C5" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Deku GITD</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -490,7 +509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="A2:E2"/>
@@ -561,7 +580,34 @@
         <v>10.01</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1"/>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="2" t="n">
+        <v>44853</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>All Might</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>17.99</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>-2.989999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding to inventory now works, requires proper grid placement
</commit_message>
<xml_diff>
--- a/Test Excel.xlsx
+++ b/Test Excel.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-7575" yWindow="4185" windowWidth="7680" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Daily Amazon" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pay Period" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mom Cost" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Daily Amazon" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Pay Period" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Mom Cost" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -735,6 +735,23 @@
       </c>
       <c r="C24" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>goku</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updating quantities, and organized inventory update window
</commit_message>
<xml_diff>
--- a/Test Excel.xlsx
+++ b/Test Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-7575" yWindow="4185" windowWidth="7680" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,15 +12,14 @@
     <sheet name="Mom Cost" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -57,11 +56,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +403,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -518,7 +516,7 @@
         <v>4.9</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -619,139 +617,92 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Isabela</t>
+          <t>Killua w/ Yoyo</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+        <v>17.99</v>
+      </c>
+      <c r="C16" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Naruto with Rasengan</t>
+          <t>Deku Glow</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+        <v>23</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Killua w/ Yoyo</t>
+          <t>Moon Knight Glow</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>17.99</v>
       </c>
       <c r="C18" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Deku Glow</t>
+          <t>Komugi</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>23</v>
+        <v>16.99</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Moon Knight Glow</t>
+          <t>2 Spiderman</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>17.99</v>
+        <v>18.72</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Komugi</t>
+          <t>Tracksuit Jerry</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>16.99</v>
+        <v>15.99</v>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2 Spiderman</t>
+          <t>Doctor Strange GITD</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>18.72</v>
+        <v>17.9</v>
       </c>
       <c r="C22" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Tracksuit Jerry</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>15.99</v>
-      </c>
-      <c r="C23" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Doctor Strange GITD</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>17.9</v>
-      </c>
-      <c r="C24" t="n">
         <v>4</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>goku</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -768,7 +719,7 @@
   </sheetPr>
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="111" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="111" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
@@ -2254,7 +2205,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="n">
+      <c r="A65" s="1" t="n">
         <v>44918</v>
       </c>
       <c r="B65" t="inlineStr">
@@ -2279,7 +2230,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="3" t="n">
+      <c r="A66" s="1" t="n">
         <v>44918</v>
       </c>
       <c r="B66" t="inlineStr">
@@ -2292,7 +2243,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="n">
+      <c r="A67" s="1" t="n">
         <v>44918</v>
       </c>
       <c r="B67" t="inlineStr">

</xml_diff>

<commit_message>
Added and orgranized entering sales, along with showing the 3 previous sales
</commit_message>
<xml_diff>
--- a/Test Excel.xlsx
+++ b/Test Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-12945" yWindow="0" windowWidth="7680" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -405,8 +405,8 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -717,10 +717,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="111" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2265,6 +2265,72 @@
       </c>
       <c r="G67" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Gotenks</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>34.99</v>
+      </c>
+      <c r="D68" t="n">
+        <v>12.11</v>
+      </c>
+      <c r="E68" t="n">
+        <v>2</v>
+      </c>
+      <c r="F68" t="n">
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Gotenks</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>34.99</v>
+      </c>
+      <c r="D69" t="n">
+        <v>12.11</v>
+      </c>
+      <c r="E69" t="n">
+        <v>2</v>
+      </c>
+      <c r="F69" t="n">
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Gotenks</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>34.99</v>
+      </c>
+      <c r="D70" t="n">
+        <v>12.11</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" t="n">
+        <v>20.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed user item input to a dropdown menu with all the items in inventory
</commit_message>
<xml_diff>
--- a/Test Excel.xlsx
+++ b/Test Excel.xlsx
@@ -723,7 +723,7 @@
       <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="10.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="20.140625" customWidth="1" min="2" max="2"/>
@@ -2351,7 +2351,7 @@
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="10.140625" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>

</xml_diff>

<commit_message>
Enter Sales working, must add designated sale
</commit_message>
<xml_diff>
--- a/Test Excel.xlsx
+++ b/Test Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-12945" yWindow="0" windowWidth="7680" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -719,13 +719,13 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:G74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="20.140625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -2351,7 +2351,7 @@
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10.140625" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>

</xml_diff>